<commit_message>
Results of SUBSEQ under Tree_expansion; see previous commit too
</commit_message>
<xml_diff>
--- a/final_experiments_data_with__SUBSEQ_tree_expansion_performance.xlsx
+++ b/final_experiments_data_with__SUBSEQ_tree_expansion_performance.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/rafaelktistakis/Repositories/sBP/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9A945680-87BF-3743-8021-5A3C13FC39F0}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B4ADA39B-6DFA-2E47-A843-9A0FE1C31039}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="51200" windowHeight="28800" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="51200" yWindow="7200" windowWidth="38400" windowHeight="21600" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Accuracy %" sheetId="1" r:id="rId1"/>
@@ -91,7 +91,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="275" uniqueCount="87">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="312" uniqueCount="90">
   <si>
     <t>DG</t>
   </si>
@@ -348,19 +348,30 @@
     <t>CPT/SUBSEQ</t>
   </si>
   <si>
-    <t>These experiments still reflect the old SUBSEQ (as was published); We need to repeat with the Tree_Expansion Version</t>
+    <t>Left are the results from PUBLISHED SUBSEQ</t>
   </si>
   <si>
-    <t>Remove comment below when numbers are updated</t>
+    <t>Right are from the Tree_Expansion_testing_performance</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> </t>
+  </si>
+  <si>
+    <t>Unchanged</t>
+  </si>
+  <si>
+    <t>The experiments we repeated on the right, were run under the same training/queries datasets as we had exported for experiments on the left. We kept the same variables as before. The only change lies on the tree_expansion mechanism that we included in our prediction phase. Nothing else got changed. Accuracy evaluation was not and is not performed for the QUEST data points.</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="2">
+  <numFmts count="4">
     <numFmt numFmtId="164" formatCode="0.0"/>
     <numFmt numFmtId="165" formatCode="0.000"/>
+    <numFmt numFmtId="169" formatCode="0.00000"/>
+    <numFmt numFmtId="170" formatCode="0.0000"/>
   </numFmts>
   <fonts count="8" x14ac:knownFonts="1">
     <font>
@@ -456,7 +467,7 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="22">
+  <cellXfs count="27">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -486,8 +497,19 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="169" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="170" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="5">
@@ -25565,7 +25587,7 @@
   <dimension ref="A1:X31"/>
   <sheetViews>
     <sheetView zoomScale="107" zoomScaleNormal="140" zoomScalePageLayoutView="140" workbookViewId="0">
-      <selection activeCell="F30" sqref="F30"/>
+      <selection activeCell="F7" sqref="F7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -26282,7 +26304,7 @@
   <dimension ref="A1:Q8"/>
   <sheetViews>
     <sheetView zoomScale="115" workbookViewId="0">
-      <selection activeCell="F10" sqref="F10"/>
+      <selection activeCell="F7" sqref="F7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -28479,7 +28501,7 @@
   <dimension ref="A1:O43"/>
   <sheetViews>
     <sheetView zoomScale="142" zoomScaleNormal="142" zoomScalePageLayoutView="142" workbookViewId="0">
-      <selection activeCell="F2" sqref="F2"/>
+      <selection activeCell="A29" sqref="A29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -29950,10 +29972,10 @@
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
-  <dimension ref="A1:G28"/>
+  <dimension ref="A1:U28"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L31" sqref="L31"/>
+      <selection activeCell="H29" sqref="H29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -29961,7 +29983,7 @@
     <col min="1" max="1" width="21.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A1" s="15" t="s">
         <v>57</v>
       </c>
@@ -29983,8 +30005,32 @@
       <c r="G1" s="15" t="s">
         <v>66</v>
       </c>
+      <c r="I1" s="15" t="s">
+        <v>85</v>
+      </c>
+      <c r="O1" s="15" t="s">
+        <v>57</v>
+      </c>
+      <c r="P1" s="15" t="s">
+        <v>61</v>
+      </c>
+      <c r="Q1" s="15" t="s">
+        <v>62</v>
+      </c>
+      <c r="R1" s="15" t="s">
+        <v>63</v>
+      </c>
+      <c r="S1" s="15" t="s">
+        <v>64</v>
+      </c>
+      <c r="T1" s="15" t="s">
+        <v>65</v>
+      </c>
+      <c r="U1" s="15" t="s">
+        <v>66</v>
+      </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>55</v>
       </c>
@@ -30006,8 +30052,22 @@
       <c r="G2" s="3">
         <v>4.5786499999999997</v>
       </c>
+      <c r="I2" t="s">
+        <v>86</v>
+      </c>
+      <c r="O2" t="s">
+        <v>55</v>
+      </c>
+      <c r="P2" s="25" t="s">
+        <v>88</v>
+      </c>
+      <c r="Q2" s="25"/>
+      <c r="R2" s="25"/>
+      <c r="S2" s="25"/>
+      <c r="T2" s="25"/>
+      <c r="U2" s="25"/>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>56</v>
       </c>
@@ -30029,8 +30089,29 @@
       <c r="G3" s="3">
         <v>0.97730600000000001</v>
       </c>
+      <c r="O3" t="s">
+        <v>56</v>
+      </c>
+      <c r="P3" s="22">
+        <v>8.0549999999999997E-3</v>
+      </c>
+      <c r="Q3" s="22">
+        <v>7.1929999999999997E-3</v>
+      </c>
+      <c r="R3" s="22">
+        <v>6.7819999999999998E-3</v>
+      </c>
+      <c r="S3" s="22">
+        <v>8.6689999999999996E-3</v>
+      </c>
+      <c r="T3" s="22">
+        <v>9.9039999999999996E-3</v>
+      </c>
+      <c r="U3" s="22">
+        <v>8.0759999999999998E-3</v>
+      </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>58</v>
       </c>
@@ -30052,8 +30133,35 @@
       <c r="G4" s="3">
         <v>8.70336</v>
       </c>
+      <c r="O4" t="s">
+        <v>58</v>
+      </c>
+      <c r="P4" s="25" t="s">
+        <v>88</v>
+      </c>
+      <c r="Q4" s="25"/>
+      <c r="R4" s="25"/>
+      <c r="S4" s="25"/>
+      <c r="T4" s="25"/>
+      <c r="U4" s="25"/>
     </row>
-    <row r="7" spans="1:7" ht="32" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="I5" s="26" t="s">
+        <v>89</v>
+      </c>
+      <c r="J5" s="26"/>
+      <c r="K5" s="26"/>
+      <c r="L5" s="26"/>
+      <c r="M5" s="26"/>
+    </row>
+    <row r="6" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="I6" s="26"/>
+      <c r="J6" s="26"/>
+      <c r="K6" s="26"/>
+      <c r="L6" s="26"/>
+      <c r="M6" s="26"/>
+    </row>
+    <row r="7" spans="1:21" ht="34" x14ac:dyDescent="0.2">
       <c r="A7" s="15" t="s">
         <v>60</v>
       </c>
@@ -30069,8 +30177,28 @@
       <c r="E7" s="18" t="s">
         <v>67</v>
       </c>
+      <c r="I7" s="26"/>
+      <c r="J7" s="26"/>
+      <c r="K7" s="26"/>
+      <c r="L7" s="26"/>
+      <c r="M7" s="26"/>
+      <c r="O7" s="15" t="s">
+        <v>60</v>
+      </c>
+      <c r="P7" s="18" t="s">
+        <v>70</v>
+      </c>
+      <c r="Q7" s="18" t="s">
+        <v>69</v>
+      </c>
+      <c r="R7" s="18" t="s">
+        <v>68</v>
+      </c>
+      <c r="S7" s="18" t="s">
+        <v>67</v>
+      </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>55</v>
       </c>
@@ -30086,8 +30214,22 @@
       <c r="E8" s="17">
         <v>4.3745700000000003</v>
       </c>
+      <c r="I8" s="26"/>
+      <c r="J8" s="26"/>
+      <c r="K8" s="26"/>
+      <c r="L8" s="26"/>
+      <c r="M8" s="26"/>
+      <c r="O8" t="s">
+        <v>55</v>
+      </c>
+      <c r="P8" s="24" t="s">
+        <v>88</v>
+      </c>
+      <c r="Q8" s="24"/>
+      <c r="R8" s="24"/>
+      <c r="S8" s="24"/>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>56</v>
       </c>
@@ -30103,8 +30245,28 @@
       <c r="E9" s="17">
         <v>7.2503999999999999E-2</v>
       </c>
+      <c r="I9" s="26"/>
+      <c r="J9" s="26"/>
+      <c r="K9" s="26"/>
+      <c r="L9" s="26"/>
+      <c r="M9" s="26"/>
+      <c r="O9" t="s">
+        <v>56</v>
+      </c>
+      <c r="P9" s="22">
+        <v>3.3939999999999999E-3</v>
+      </c>
+      <c r="Q9" s="22">
+        <v>3.676E-3</v>
+      </c>
+      <c r="R9" s="22">
+        <v>6.0590000000000001E-3</v>
+      </c>
+      <c r="S9" s="22">
+        <v>1.3009E-2</v>
+      </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>58</v>
       </c>
@@ -30120,8 +30282,29 @@
       <c r="E10" s="17">
         <v>6.6927099999999999</v>
       </c>
+      <c r="I10" s="26"/>
+      <c r="J10" s="26"/>
+      <c r="K10" s="26"/>
+      <c r="L10" s="26"/>
+      <c r="M10" s="26"/>
+      <c r="O10" t="s">
+        <v>58</v>
+      </c>
+      <c r="P10" s="24" t="s">
+        <v>88</v>
+      </c>
+      <c r="Q10" s="24"/>
+      <c r="R10" s="24"/>
+      <c r="S10" s="24"/>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="I11" s="26"/>
+      <c r="J11" s="26"/>
+      <c r="K11" s="26"/>
+      <c r="L11" s="26"/>
+      <c r="M11" s="26"/>
+    </row>
+    <row r="12" spans="1:21" ht="34" x14ac:dyDescent="0.2">
       <c r="A12" s="16" t="s">
         <v>59</v>
       </c>
@@ -30140,8 +30323,31 @@
       <c r="F12" s="18" t="s">
         <v>73</v>
       </c>
+      <c r="I12" s="26"/>
+      <c r="J12" s="26"/>
+      <c r="K12" s="26"/>
+      <c r="L12" s="26"/>
+      <c r="M12" s="26"/>
+      <c r="O12" s="16" t="s">
+        <v>59</v>
+      </c>
+      <c r="P12" s="18" t="s">
+        <v>74</v>
+      </c>
+      <c r="Q12" s="18" t="s">
+        <v>75</v>
+      </c>
+      <c r="R12" s="18" t="s">
+        <v>71</v>
+      </c>
+      <c r="S12" s="18" t="s">
+        <v>72</v>
+      </c>
+      <c r="T12" s="18" t="s">
+        <v>73</v>
+      </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A13" s="11" t="s">
         <v>55</v>
       </c>
@@ -30160,8 +30366,18 @@
       <c r="F13" s="3">
         <v>12.366899999999999</v>
       </c>
+      <c r="O13" s="11" t="s">
+        <v>55</v>
+      </c>
+      <c r="P13" s="25" t="s">
+        <v>88</v>
+      </c>
+      <c r="Q13" s="25"/>
+      <c r="R13" s="25"/>
+      <c r="S13" s="25"/>
+      <c r="T13" s="25"/>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A14" s="11" t="s">
         <v>56</v>
       </c>
@@ -30180,8 +30396,26 @@
       <c r="F14" s="3">
         <v>14.345499999999999</v>
       </c>
+      <c r="O14" s="11" t="s">
+        <v>56</v>
+      </c>
+      <c r="P14" s="21">
+        <v>7.7099999999999998E-4</v>
+      </c>
+      <c r="Q14" s="21">
+        <v>1.2719999999999999E-3</v>
+      </c>
+      <c r="R14" s="21">
+        <v>2.431E-3</v>
+      </c>
+      <c r="S14" s="21">
+        <v>4.9319999999999998E-3</v>
+      </c>
+      <c r="T14" s="21">
+        <v>1.0858E-2</v>
+      </c>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A15" s="11" t="s">
         <v>58</v>
       </c>
@@ -30200,8 +30434,18 @@
       <c r="F15" s="3">
         <v>18.892600000000002</v>
       </c>
+      <c r="O15" s="11" t="s">
+        <v>58</v>
+      </c>
+      <c r="P15" s="25" t="s">
+        <v>88</v>
+      </c>
+      <c r="Q15" s="25"/>
+      <c r="R15" s="25"/>
+      <c r="S15" s="25"/>
+      <c r="T15" s="25"/>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A18" s="16" t="s">
         <v>76</v>
       </c>
@@ -30214,8 +30458,20 @@
       <c r="D18" s="3">
         <v>12</v>
       </c>
+      <c r="O18" s="16" t="s">
+        <v>76</v>
+      </c>
+      <c r="P18" s="3">
+        <v>3</v>
+      </c>
+      <c r="Q18" s="3">
+        <v>6</v>
+      </c>
+      <c r="R18" s="3">
+        <v>12</v>
+      </c>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A19" s="11" t="s">
         <v>77</v>
       </c>
@@ -30228,18 +30484,35 @@
       <c r="D19">
         <v>1.0847500000000001</v>
       </c>
+      <c r="O19" s="11" t="s">
+        <v>77</v>
+      </c>
+      <c r="P19">
+        <v>3.1500000000000001E-4</v>
+      </c>
+      <c r="Q19">
+        <v>3.1399999999999999E-4</v>
+      </c>
+      <c r="R19">
+        <v>3.28E-4</v>
+      </c>
     </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A27" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="28" spans="1:4" ht="85" x14ac:dyDescent="0.2">
-      <c r="A28" s="21" t="s">
-        <v>85</v>
+    <row r="28" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="A28" s="23"/>
+      <c r="P28" t="s">
+        <v>87</v>
       </c>
     </row>
   </sheetData>
+  <mergeCells count="7">
+    <mergeCell ref="I5:M12"/>
+    <mergeCell ref="P8:S8"/>
+    <mergeCell ref="P10:S10"/>
+    <mergeCell ref="P4:U4"/>
+    <mergeCell ref="P2:U2"/>
+    <mergeCell ref="P13:T13"/>
+    <mergeCell ref="P15:T15"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>

</xml_diff>

<commit_message>
minor changes in the spreadsheet
</commit_message>
<xml_diff>
--- a/final_experiments_data_with__SUBSEQ_tree_expansion_performance.xlsx
+++ b/final_experiments_data_with__SUBSEQ_tree_expansion_performance.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/rafaelktistakis/Repositories/sBP/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CF69406B-D008-A644-BC61-970AC9C9FD71}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8DB1B81E-88BB-3B4E-9599-E69D6CC60818}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="51200" yWindow="7200" windowWidth="38400" windowHeight="21600" firstSheet="4" activeTab="11" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -16188,7 +16188,7 @@
           <c:idx val="1"/>
           <c:order val="1"/>
           <c:tx>
-            <c:v>subSeq Prime</c:v>
+            <c:v>SUBSEQ Prime</c:v>
           </c:tx>
           <c:spPr>
             <a:pattFill prst="diagBrick">
@@ -36071,8 +36071,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:S25"/>
   <sheetViews>
-    <sheetView zoomScale="64" zoomScaleNormal="142" zoomScalePageLayoutView="142" workbookViewId="0">
-      <selection activeCell="D38" sqref="D38"/>
+    <sheetView zoomScale="125" zoomScaleNormal="142" zoomScalePageLayoutView="142" workbookViewId="0">
+      <selection activeCell="G8" sqref="G8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -36138,7 +36138,7 @@
         <v>37</v>
       </c>
       <c r="G2" s="3">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="H2" s="4">
         <v>33</v>
@@ -36180,7 +36180,7 @@
         <v>34</v>
       </c>
       <c r="G3" s="3">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="H3" s="4">
         <v>23</v>
@@ -36306,7 +36306,7 @@
         <v>80</v>
       </c>
       <c r="G6" s="3">
-        <v>81</v>
+        <v>84</v>
       </c>
       <c r="H6" s="4">
         <v>88</v>
@@ -36348,7 +36348,7 @@
         <v>29</v>
       </c>
       <c r="G7" s="3">
-        <v>27</v>
+        <v>32</v>
       </c>
       <c r="H7" s="4">
         <v>34</v>
@@ -37006,7 +37006,7 @@
   </sheetPr>
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView zoomScale="108" workbookViewId="0">
+    <sheetView topLeftCell="F17" zoomScale="108" workbookViewId="0">
       <selection activeCell="L35" sqref="L35"/>
     </sheetView>
   </sheetViews>
@@ -37042,7 +37042,7 @@
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="60" workbookViewId="0">
-      <selection activeCell="AD44" sqref="AD44"/>
+      <selection activeCell="AJ60" sqref="AJ60"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -38997,7 +38997,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:I27"/>
   <sheetViews>
-    <sheetView zoomScale="75" zoomScaleNormal="142" zoomScalePageLayoutView="142" workbookViewId="0">
+    <sheetView zoomScale="125" zoomScaleNormal="142" zoomScalePageLayoutView="142" workbookViewId="0">
       <selection activeCell="Z13" sqref="Z13:AC40"/>
     </sheetView>
   </sheetViews>

</xml_diff>